<commit_message>
Saves vouchers to excel.
</commit_message>
<xml_diff>
--- a/NESS.VoucherManagement.Persistence.Tests/ExcelFiles/employees.xlsx
+++ b/NESS.VoucherManagement.Persistence.Tests/ExcelFiles/employees.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nadia HR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\NESS.VoucherManagement\NESS.VoucherManagement.Persistence.Tests\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="lista cnp" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -78,19 +78,19 @@
     <t>Constantin Gheorghe</t>
   </si>
   <si>
-    <t xml:space="preserve">Constantin </t>
-  </si>
-  <si>
     <t>Gheorghe</t>
   </si>
   <si>
     <t>CRISTIAN.POPESCU@NESS.COM</t>
+  </si>
+  <si>
+    <t>Constantin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -946,7 +946,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,16 +1047,16 @@
         <v>18</v>
       </c>
       <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
         <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
       </c>
       <c r="E5">
         <v>1830203115230</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>